<commit_message>
Creating unit tests for OrganiserParser. Added missing Tiebreak round format to example files.
</commit_message>
<xml_diff>
--- a/exampleFiles/Entry_Sheet.xlsx
+++ b/exampleFiles/Entry_Sheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
   <si>
     <t>Group Stage</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>H2</t>
+  </si>
+  <si>
+    <t>Tiebreak</t>
   </si>
 </sst>
 </file>
@@ -450,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,7 +467,7 @@
     <col min="7" max="7" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -480,8 +483,11 @@
       <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K1" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>5</v>
       </c>
@@ -494,8 +500,11 @@
       <c r="I2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -509,7 +518,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -520,7 +529,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -531,12 +540,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -544,7 +553,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -552,7 +561,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -560,27 +569,27 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
Added unit test for EntryParser
</commit_message>
<xml_diff>
--- a/exampleFiles/Entry_Sheet.xlsx
+++ b/exampleFiles/Entry_Sheet.xlsx
@@ -18,9 +18,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
   <si>
-    <t>Group Stage</t>
-  </si>
-  <si>
     <t>Quarter Finals</t>
   </si>
   <si>
@@ -106,6 +103,9 @@
   </si>
   <si>
     <t>Tiebreak</t>
+  </si>
+  <si>
+    <t>Qualifying</t>
   </si>
 </sst>
 </file>
@@ -455,9 +455,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -469,36 +467,36 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="K1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" t="s">
         <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" t="s">
-        <v>6</v>
       </c>
       <c r="K2">
         <v>32</v>
@@ -506,157 +504,157 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>8</v>
       </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
       <c r="G3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
         <v>10</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
         <v>14</v>
-      </c>
-      <c r="C8" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>